<commit_message>
A temp version for Layer-3
</commit_message>
<xml_diff>
--- a/Examples/ParticipationAnalysis/ModalConfig_IEEE_14Bus_Cyprus_test.xlsx
+++ b/Examples/ParticipationAnalysis/ModalConfig_IEEE_14Bus_Cyprus_test.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Git\Simplex-Power-Systems-2\Examples\ParticipationAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418A187C-2706-41DD-9CBE-A666098D1BBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB1EBA5-2734-4C94-A1FE-C9717234222D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{9ED4A44B-10E7-45E8-AE16-14F27C619C20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9ED4A44B-10E7-45E8-AE16-14F27C619C20}"/>
   </bookViews>
   <sheets>
-    <sheet name="State-PF" sheetId="10" r:id="rId1"/>
-    <sheet name="Impedance-PF" sheetId="11" r:id="rId2"/>
-    <sheet name="Enabling" sheetId="12" r:id="rId3"/>
+    <sheet name="State-PF" sheetId="19" r:id="rId1"/>
+    <sheet name="Impedance-PF" sheetId="20" r:id="rId2"/>
+    <sheet name="Enabling" sheetId="21" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2116,7 +2116,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C11E174-2011-427C-8A86-5955177CA49C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543101C4-489D-4594-88DE-73299C4A7BA1}">
   <dimension ref="A1:G293"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7058,14 +7058,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A0C4F1B-AC06-4167-8EA5-53A2F5ECE8AD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77CAC62A-8601-4C9E-B5AE-B595CB3D6739}">
   <dimension ref="A1:L294"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:L294"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I157" sqref="I157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="22.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -7146,7 +7150,7 @@
         <v>7</v>
       </c>
       <c r="L8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -7256,7 +7260,7 @@
         <v>155</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -9500,7 +9504,7 @@
         <v>436</v>
       </c>
       <c r="I216">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="217" spans="7:9" x14ac:dyDescent="0.25">
@@ -10367,11 +10371,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9BA1E24-FFF2-4A89-BA35-67E804CAD735}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F9E4E2-4878-4F18-BEB8-7C1FE3B63B9D}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10399,7 +10403,7 @@
         <v>572</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -10407,7 +10411,7 @@
         <v>573</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>